<commit_message>
Add function class section management for teacher - View list class section - View add suggested TA
</commit_message>
<xml_diff>
--- a/Content/Uploads/ImportTKB/ThoiKhoaBieu_TieuChuan_Mau.xlsx
+++ b/Content/Uploads/ImportTKB/ThoiKhoaBieu_TieuChuan_Mau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\CAPSTONE2024-DOCX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79A626F-6FCB-4709-98A5-6B34A866221C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14DA2B7-FDD8-4CC2-9B31-134B8F3B01DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1469,10 +1469,10 @@
   <dimension ref="A1:AF31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1494,7 +1494,7 @@
     <col min="26" max="26" width="21.3984375" customWidth="1"/>
     <col min="27" max="27" width="21.59765625" customWidth="1"/>
     <col min="28" max="28" width="23.296875" customWidth="1"/>
-    <col min="29" max="29" width="9.09765625" customWidth="1"/>
+    <col min="29" max="29" width="12.5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12.8984375" customWidth="1"/>
     <col min="31" max="31" width="16.296875" style="2" customWidth="1"/>
     <col min="32" max="32" width="17.69921875" customWidth="1"/>

</xml_diff>